<commit_message>
Chipping away at the custom attribute icons. All the multi-Attribute icons are done, all the readability aids are setup, now to export the mockups.
</commit_message>
<xml_diff>
--- a/Custom Cards/Category - Custom Mechanics (Design & Demo)/Multi-Attribute Monsters/Designs/Attribute Combinations.xlsx
+++ b/Custom Cards/Category - Custom Mechanics (Design & Demo)/Multi-Attribute Monsters/Designs/Attribute Combinations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Category - Custom Mechanics (Design &amp; Demo)\Multi-Attribute Monsters\Images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Category - Custom Mechanics (Design &amp; Demo)\Multi-Attribute Monsters\Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4ED12E-147A-457D-85CE-9937472FA2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94B8EA4-066D-42C6-9C11-25F8C2E547EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="4" xr2:uid="{AD9CF55C-5A2C-43F9-8449-28DA4DBE7F5E}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="76">
   <si>
     <t>EARTH</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>WATER/FIRE/WIND/DARK</t>
+  </si>
+  <si>
+    <t>EARTH/WATER/LIGHT/DARK</t>
   </si>
 </sst>
 </file>
@@ -261,7 +264,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -300,12 +303,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1396,7 +1400,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1432,7 +1436,7 @@
       <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D2" t="s">
@@ -1449,7 +1453,7 @@
       <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D3" t="s">
@@ -1463,7 +1467,7 @@
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>60</v>
       </c>
       <c r="D4" t="s">
@@ -1477,7 +1481,7 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D5" t="s">
@@ -1491,7 +1495,7 @@
       <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>63</v>
       </c>
       <c r="D6" t="s">
@@ -1505,8 +1509,8 @@
       <c r="B7" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
-        <v>70</v>
+      <c r="C7" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="D7" t="s">
         <v>52</v>
@@ -1519,7 +1523,7 @@
       <c r="B8" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1530,7 +1534,7 @@
       <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1541,7 +1545,7 @@
       <c r="B10" t="s">
         <v>41</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1552,7 +1556,7 @@
       <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1563,7 +1567,7 @@
       <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1574,7 +1578,7 @@
       <c r="B13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1585,7 +1589,7 @@
       <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1596,7 +1600,7 @@
       <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1607,7 +1611,7 @@
       <c r="B16" t="s">
         <v>31</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>